<commit_message>
Finished board and BoM
</commit_message>
<xml_diff>
--- a/E&S_Datalogger/ES_Datalogger_BOM.xlsx
+++ b/E&S_Datalogger/ES_Datalogger_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -19,25 +19,178 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>3.3V Reg</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/rohm-semiconductor/BD33KA5FP-E2/BD33KA5FP-E2CT-ND/3663779</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>https://www.digikey.com/product-detail/en/molex-llc/0548190519/WM17115-ND/773802</t>
   </si>
   <si>
-    <t>Mini USB</t>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>3.3V Regulator</t>
+  </si>
+  <si>
+    <t>Female MiniUSB Header</t>
+  </si>
+  <si>
+    <t>SAMD21</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATSAMD21G18A-AUT/ATSAMD21G18A-AUTCT-ND/4878879</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>32.782kHz</t>
+  </si>
+  <si>
+    <t>Might want to look into cheaper packages</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/epson/MC-156-32.7680KA-A0-ROHS/SER2412CT-ND/1532558</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/GCM21BR72A104KA37K/490-8051-1-ND/4380336</t>
+  </si>
+  <si>
+    <t>15pF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/samsung-electro-mechanics/CL21C150JBANNNC/1276-1163-1-ND/3889249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor </t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/RNCF0805DTE10K0/RNCF0805DTE10K0CT-ND/2687083</t>
+  </si>
+  <si>
+    <t>CORTEX Debug</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cnc-tech/3220-10-0100-00/1175-1627-ND/3883661</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/diodes-incorporated/AP2112K-3.3TRG1/AP2112K-3.3TRG1DICT-ND/4505257</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>JST Connector</t>
+  </si>
+  <si>
+    <t>SD Card Holder</t>
+  </si>
+  <si>
+    <t>Micro SD Card</t>
+  </si>
+  <si>
+    <t>MPU 9250</t>
+  </si>
+  <si>
+    <t>MPL3115A2</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Yellow LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/yageo/CC0805ZKY5V6BB106/311-1355-1-ND/2103139</t>
+  </si>
+  <si>
+    <t>LiPo Battery</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/13813</t>
+  </si>
+  <si>
+    <t>1Ah</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8612</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/advantech-corp/SQF-MSDM1-4G-21C/SQF-MSDM1-4G-21C-ND/6614433</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-invensense/MPU-9250/1428-1019-1-ND/4626450</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/nxp-usa-inc/MPL3115A2/MPL3115A2-ND/2817529</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-llc/5031821852/WM12834CT-ND/5823232</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8720</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C171GKT/160-1423-1-ND/386792</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C171KSKT/160-1428-1-ND/386802</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lite-on-inc/LTST-C171KRKT/160-1427-1-ND/386800</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERA-6AEB101V/P100DACT-ND/1465923</t>
+  </si>
+  <si>
+    <t>We have some of these</t>
+  </si>
+  <si>
+    <t>We have these</t>
+  </si>
+  <si>
+    <t>Got these</t>
+  </si>
+  <si>
+    <t>Might want to order one just in case, we can go a size smaller too</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +206,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -62,7 +240,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,18 +248,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,37 +561,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="35.77734375" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="6" max="6" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4">
         <v>2</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F5" r:id="rId5"/>
+    <hyperlink ref="F4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>